<commit_message>
correcciones en el metricas converter
</commit_message>
<xml_diff>
--- a/carbono/src/test/resources/sample2.xlsx
+++ b/carbono/src/test/resources/sample2.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanUTN\carbono\carbono\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C938356-CB2C-4B1E-B509-A55AB7D9EFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="1740" yWindow="1365" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>Actividad</t>
   </si>
@@ -51,9 +57,6 @@
     <t>Combustión Móvil</t>
   </si>
   <si>
-    <t>Combustible consumido nafta</t>
-  </si>
-  <si>
     <t>MENSUAL</t>
   </si>
   <si>
@@ -66,18 +69,12 @@
     <t>Lógistica de productos y servicios</t>
   </si>
   <si>
-    <t>Peso total transportado</t>
-  </si>
-  <si>
     <t>GNC</t>
   </si>
   <si>
     <t>Carbón</t>
   </si>
   <si>
-    <t>Residuos</t>
-  </si>
-  <si>
     <t>Gasoil</t>
   </si>
   <si>
@@ -87,24 +84,9 @@
     <t>Distancia</t>
   </si>
   <si>
-    <t>Materia Prima</t>
-  </si>
-  <si>
     <t>2022</t>
   </si>
   <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>Kerosene</t>
-  </si>
-  <si>
-    <t>Productos</t>
-  </si>
-  <si>
-    <t>Utilitario Liviano</t>
-  </si>
-  <si>
     <t>11/2021</t>
   </si>
   <si>
@@ -126,17 +108,32 @@
     <t>10/2022</t>
   </si>
   <si>
-    <t>05/2022</t>
-  </si>
-  <si>
     <t>04/2022</t>
+  </si>
+  <si>
+    <t>Logistica de productos y servicios</t>
+  </si>
+  <si>
+    <t>peso</t>
+  </si>
+  <si>
+    <t>categoria</t>
+  </si>
+  <si>
+    <t>medio_transporte</t>
+  </si>
+  <si>
+    <t>utilitario liviano</t>
+  </si>
+  <si>
+    <t>materia prima</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +165,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -260,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -278,6 +289,13 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -568,18 +586,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,30 +610,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="10"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -628,10 +646,10 @@
         <v>1000</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -639,254 +657,203 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" s="4">
         <v>20</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="C5" s="4">
         <v>200</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4">
-        <v>2000</v>
+        <v>250</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="4">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4">
+        <v>260</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="4">
-        <v>100</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="4">
-        <v>260</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>32</v>
+      <c r="C9" s="8">
+        <v>150</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="4">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C11" s="4">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C12" s="4">
         <v>1000</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C13" s="4">
-        <v>15000</v>
+        <v>100</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>24</v>
+        <v>10</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="4">
-        <v>100</v>
+        <v>30</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="4">
-        <v>1000</v>
+        <v>31</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="4">
-        <v>100</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="4">
-        <v>100</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C18" s="4">
-        <v>10000</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -899,7 +866,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="E10 E18 E12:E13" numberStoredAsText="1"/>
+    <ignoredError sqref="E10" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>